<commit_message>
Use addressable to spawn the dialog and button + more dialog excel info
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterDialogUI.xlsx
+++ b/Assets/Data/Excel/MasterDialogUI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A8CC9F-44F5-46DB-BA33-E8C9FAE74FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4BF670-F1FA-4EDD-A39F-8A46CE24F91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Do you want to reset the current tab back to default value?</t>
   </si>
   <si>
-    <t>YesNo</t>
-  </si>
-  <si>
     <t>description_EN</t>
   </si>
   <si>
@@ -67,13 +64,38 @@
   </si>
   <si>
     <t>buttonDisplayType</t>
+  </si>
+  <si>
+    <t>widthRatio</t>
+  </si>
+  <si>
+    <t>heightRatio</t>
+  </si>
+  <si>
+    <t>Two_YesNo</t>
+  </si>
+  <si>
+    <t>buttonAText</t>
+  </si>
+  <si>
+    <t>buttonBText</t>
+  </si>
+  <si>
+    <t>buttonCText</t>
+  </si>
+  <si>
+    <t>dialogueUIType, dialogDisplayType, buttonDisplayType are enum.
+widthRatio/heightRatio are from 0~1.
+If buttonText are not written, it will use the default text.
+title_EN is the title on the dialogBox.
+description_EN is the desctiption to the player.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,16 +103,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -98,15 +140,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -418,42 +483,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E91137-7BD2-48ED-A93D-3ECC6F638E0D}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="72.5546875" customWidth="1"/>
-    <col min="5" max="5" width="28.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="55.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -461,17 +549,35 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>0.3</v>
+      </c>
+      <c r="I2">
+        <v>0.3</v>
+      </c>
+      <c r="J2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="K2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>